<commit_message>
CCDB-202: The property association removed. Removed the integration tests for associations. Fixed a bug in data loaders revealed by the removal.
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/duplicate-field-failure-test.xlsx
+++ b/conf-core/src/test/resources/dataloader/duplicate-field-failure-test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>HEADER</t>
   </si>
@@ -32,9 +32,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>ASSOCIATION</t>
-  </si>
-  <si>
     <t>UNIT</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>association</t>
-  </si>
-  <si>
     <t>units</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
   </si>
   <si>
     <t>Accumulated Center Position</t>
-  </si>
-  <si>
-    <t>SLOT</t>
   </si>
   <si>
     <t>meter</t>
@@ -413,20 +404,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,51 +438,42 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>